<commit_message>
Controls added. Improved UI
</commit_message>
<xml_diff>
--- a/Week 1 Assignment - Dungeon Crawler/data/Data Sheet.xlsx
+++ b/Week 1 Assignment - Dungeon Crawler/data/Data Sheet.xlsx
@@ -5,15 +5,16 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemo1\Source\Repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemo1\source\repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3D9C21F1-9C80-43D5-8AF9-6D5746E36896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DE9ED40-1ACC-403F-B0C3-2E68D803ED89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Rooms" sheetId="1" r:id="rId1"/>
+    <sheet name="Items" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,14 +27,17 @@
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{EB932CA5-92BA-46AE-82AA-E9F012A5E1C2}" name="room_schema" type="4" refreshedVersion="0" background="1">
+  <connection id="1" xr16:uid="{4C6AA9E1-8172-4EC5-B671-5905627E9369}" name="item_schema" type="4" refreshedVersion="0" background="1">
+    <webPr xml="1" sourceData="1" url="C:\Users\nemo1\source\repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\Schema\item_schema.xml" htmlTables="1" htmlFormat="all"/>
+  </connection>
+  <connection id="2" xr16:uid="{EB932CA5-92BA-46AE-82AA-E9F012A5E1C2}" name="room_schema" type="4" refreshedVersion="0" background="1">
     <webPr xml="1" sourceData="1" url="C:\Users\nemo1\source\repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\Schema\room_schema.xml" htmlTables="1" htmlFormat="all"/>
   </connection>
 </connections>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="37">
   <si>
     <t>ID</t>
   </si>
@@ -102,6 +106,48 @@
   </si>
   <si>
     <t>A Wall</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>LocationID</t>
+  </si>
+  <si>
+    <t>Flashlight</t>
+  </si>
+  <si>
+    <t>A black flashlight</t>
+  </si>
+  <si>
+    <t>Crayon</t>
+  </si>
+  <si>
+    <t>A red crayon</t>
+  </si>
+  <si>
+    <t>Rope</t>
+  </si>
+  <si>
+    <t>Some rope</t>
+  </si>
+  <si>
+    <t>Weed</t>
+  </si>
+  <si>
+    <t>A jar of weed</t>
+  </si>
+  <si>
+    <t>Knife</t>
+  </si>
+  <si>
+    <t>A karambit</t>
+  </si>
+  <si>
+    <t>Banjo</t>
+  </si>
+  <si>
+    <t>An old banjo with a missing string.</t>
   </si>
 </sst>
 </file>
@@ -187,14 +233,36 @@
       </xsd:element>
     </xsd:schema>
   </Schema>
+  <Schema ID="Schema2">
+    <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns="">
+      <xsd:element nillable="true" name="Item-data">
+        <xsd:complexType>
+          <xsd:sequence minOccurs="0">
+            <xsd:element minOccurs="0" maxOccurs="unbounded" nillable="true" name="Item" form="unqualified">
+              <xsd:complexType>
+                <xsd:sequence minOccurs="0">
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Name" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="Description" form="unqualified"/>
+                  <xsd:element minOccurs="0" nillable="true" type="xsd:string" name="LocationID" form="unqualified"/>
+                </xsd:sequence>
+              </xsd:complexType>
+            </xsd:element>
+          </xsd:sequence>
+        </xsd:complexType>
+      </xsd:element>
+    </xsd:schema>
+  </Schema>
+  <Map ID="6" Name="Item-data_Map" RootElement="Item-data" SchemaID="Schema2" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
+    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+  </Map>
   <Map ID="5" Name="Room-data_Map" RootElement="Room-data" SchemaID="Schema1" ShowImportExportValidationErrors="false" AutoFit="true" Append="false" PreserveSortAFLayout="true" PreserveFormat="true">
-    <DataBinding FileBinding="true" ConnectionID="1" DataBindingLoadMode="1"/>
+    <DataBinding FileBinding="true" ConnectionID="2" DataBindingLoadMode="1"/>
   </Map>
 </MapInfo>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C7C18A-8ED5-40AC-87CA-DF359B1674B0}" name="Table1" displayName="Table1" ref="A1:K7" tableType="xml" totalsRowShown="0" connectionId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{33C7C18A-8ED5-40AC-87CA-DF359B1674B0}" name="Table1" displayName="Table1" ref="A1:K7" tableType="xml" totalsRowShown="0" connectionId="2">
   <autoFilter ref="A1:K7" xr:uid="{33C7C18A-8ED5-40AC-87CA-DF359B1674B0}"/>
   <tableColumns count="11">
     <tableColumn id="1" xr3:uid="{91FD8FE9-892C-4567-B773-8894F10150AE}" uniqueName="ID" name="ID">
@@ -229,6 +297,24 @@
     </tableColumn>
     <tableColumn id="11" xr3:uid="{2DCCDC6D-7213-4779-9D4D-83951F9CFEA5}" uniqueName="wTrapID" name="wTrapID">
       <xmlColumnPr mapId="5" xpath="/Room-data/Room/wTrapID" xmlDataType="integer"/>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{61E3FEA6-0EE3-4067-A678-43359193BFC4}" name="Table2" displayName="Table2" ref="A1:C7" tableType="xml" totalsRowShown="0" connectionId="1">
+  <autoFilter ref="A1:C7" xr:uid="{61E3FEA6-0EE3-4067-A678-43359193BFC4}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{72BF0D12-7B32-4E3B-86E7-947970E49766}" uniqueName="Name" name="Name">
+      <xmlColumnPr mapId="6" xpath="/Item-data/Item/Name" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="2" xr3:uid="{C18329BE-64D2-4973-BEF2-EE338068153C}" uniqueName="Description" name="Description">
+      <xmlColumnPr mapId="6" xpath="/Item-data/Item/Description" xmlDataType="string"/>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{1B22A37A-3F3D-49DE-8483-D588BD7E6B98}" uniqueName="LocationID" name="LocationID">
+      <xmlColumnPr mapId="6" xpath="/Item-data/Item/LocationID" xmlDataType="string"/>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -500,8 +586,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -553,7 +639,7 @@
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2">
         <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
@@ -588,7 +674,7 @@
       </c>
     </row>
     <row r="3" spans="1:11" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
@@ -760,6 +846,106 @@
       </c>
       <c r="K7">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88530C06-13D6-4395-8D77-2941F18E7D74}">
+  <dimension ref="A1:C7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="24.44140625" customWidth="1"/>
+    <col min="2" max="2" width="32.88671875" customWidth="1"/>
+    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C2" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>31</v>
+      </c>
+      <c r="B5" t="s">
+        <v>32</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
JS Node Added (Wk5)
</commit_message>
<xml_diff>
--- a/Week 1 Assignment - Dungeon Crawler/data/Data Sheet.xlsx
+++ b/Week 1 Assignment - Dungeon Crawler/data/Data Sheet.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26731"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nemo1\Source\Repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cedillo02\Source\Repos\Glareyo\Prog-340-GraphicsApplicationProgramming\Week 1 Assignment - Dungeon Crawler\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{169EAF6A-7FA5-4620-92A0-5BECE3BA84D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A87B9DAF-079E-4F7C-9A81-F1096300D463}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Rooms" sheetId="1" r:id="rId1"/>
@@ -1049,20 +1049,20 @@
       <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" style="4" customWidth="1"/>
-    <col min="2" max="2" width="21.21875" customWidth="1"/>
-    <col min="3" max="3" width="40.6640625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="9.88671875" customWidth="1"/>
-    <col min="5" max="7" width="8.88671875" customWidth="1"/>
-    <col min="8" max="8" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.7109375" style="4" customWidth="1"/>
+    <col min="2" max="2" width="21.28515625" customWidth="1"/>
+    <col min="3" max="3" width="40.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="9.85546875" customWidth="1"/>
+    <col min="5" max="7" width="8.85546875" customWidth="1"/>
+    <col min="8" max="8" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -1088,7 +1088,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5">
         <v>0</v>
       </c>
@@ -1114,7 +1114,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="54" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1140,7 +1140,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="52.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:8" ht="52.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="5">
         <v>2</v>
       </c>
@@ -1166,7 +1166,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="43.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:8" ht="43.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="5">
         <v>3</v>
       </c>
@@ -1192,7 +1192,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
         <v>4</v>
       </c>
@@ -1218,7 +1218,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:8" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="5">
         <v>5</v>
       </c>
@@ -1244,7 +1244,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:8" ht="52.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:8" ht="52.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="4">
         <v>6</v>
       </c>
@@ -1270,7 +1270,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="4">
         <v>7</v>
       </c>
@@ -1296,7 +1296,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="4">
         <v>8</v>
       </c>
@@ -1322,7 +1322,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:8" ht="70.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:8" ht="70.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="4">
         <v>9</v>
       </c>
@@ -1348,7 +1348,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="12" spans="1:8" ht="71.400000000000006" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" ht="71.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4">
         <v>10</v>
       </c>
@@ -1374,7 +1374,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:8" ht="44.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:8" ht="44.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="4">
         <v>11</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:8" ht="60.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:8" ht="60.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="4">
         <v>12</v>
       </c>
@@ -1426,7 +1426,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="15" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:8" ht="51" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="4">
         <v>13</v>
       </c>
@@ -1452,7 +1452,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="16" spans="1:8" ht="61.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:8" ht="61.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="4">
         <v>14</v>
       </c>
@@ -1478,7 +1478,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:8" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="4">
         <v>15</v>
       </c>
@@ -1504,7 +1504,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="18" spans="1:8" ht="61.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:8" ht="61.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="4">
         <v>16</v>
       </c>
@@ -1530,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:8" ht="49.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:8" ht="49.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="4">
         <v>17</v>
       </c>
@@ -1556,7 +1556,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:8" ht="76.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:8" ht="76.150000000000006" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4">
         <v>18</v>
       </c>
@@ -1582,7 +1582,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:8" ht="85.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:8" ht="85.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="4">
         <v>19</v>
       </c>
@@ -1608,7 +1608,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="22" spans="1:8" ht="55.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:8" ht="55.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
         <v>20</v>
       </c>
@@ -1634,7 +1634,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="23" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:8" ht="45.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="4">
         <v>21</v>
       </c>
@@ -1660,7 +1660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:8" ht="46.8" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:8" ht="46.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="4">
         <v>22</v>
       </c>
@@ -1686,7 +1686,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:8" ht="63" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="4">
         <v>23</v>
       </c>
@@ -1712,7 +1712,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="26" spans="1:8" ht="56.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:8" ht="56.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4">
         <v>24</v>
       </c>
@@ -1738,7 +1738,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="27" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:8" ht="51.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="4">
         <v>25</v>
       </c>
@@ -1764,7 +1764,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="28" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="4">
         <v>26</v>
       </c>
@@ -1806,18 +1806,18 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.88671875" customWidth="1"/>
-    <col min="2" max="2" width="8.21875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="39.109375" customWidth="1"/>
-    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="1" max="1" width="13.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="24.28515625" customWidth="1"/>
     <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="29" customWidth="1"/>
-    <col min="7" max="7" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="50.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" ht="50.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1840,7 +1840,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" ht="105.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>19</v>
       </c>
@@ -1863,7 +1863,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1886,7 +1886,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1909,7 +1909,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1932,7 +1932,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1978,7 +1978,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="53.4" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:7" ht="53.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2001,7 +2001,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="37.799999999999997" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:7" ht="37.9" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2024,7 +2024,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:7" ht="54.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2047,7 +2047,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" ht="42.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2070,7 +2070,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2093,7 +2093,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="46.2" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" ht="46.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2116,7 +2116,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="117" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2152,18 +2152,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88530C06-13D6-4395-8D77-2941F18E7D74}">
   <dimension ref="A1:C20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="24.44140625" customWidth="1"/>
-    <col min="2" max="2" width="32.88671875" customWidth="1"/>
-    <col min="3" max="3" width="30.44140625" customWidth="1"/>
+    <col min="1" max="1" width="24.42578125" customWidth="1"/>
+    <col min="2" max="2" width="32.85546875" customWidth="1"/>
+    <col min="3" max="3" width="30.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -2174,7 +2174,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>68</v>
       </c>
@@ -2185,7 +2185,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>74</v>
       </c>
@@ -2196,7 +2196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>109</v>
       </c>
@@ -2207,7 +2207,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>103</v>
       </c>
@@ -2218,7 +2218,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>86</v>
       </c>
@@ -2229,7 +2229,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>142</v>
       </c>
@@ -2240,7 +2240,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>109</v>
       </c>
@@ -2251,7 +2251,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>97</v>
       </c>
@@ -2262,7 +2262,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>80</v>
       </c>
@@ -2273,7 +2273,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -2284,7 +2284,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>146</v>
       </c>
@@ -2295,7 +2295,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>147</v>
       </c>
@@ -2306,7 +2306,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>120</v>
       </c>
@@ -2317,7 +2317,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>11</v>
       </c>
@@ -2328,7 +2328,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>153</v>
       </c>
@@ -2339,7 +2339,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>74</v>
       </c>
@@ -2350,7 +2350,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>155</v>
       </c>
@@ -2361,7 +2361,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>131</v>
       </c>
@@ -2372,7 +2372,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>158</v>
       </c>

</xml_diff>